<commit_message>
Adding gitignore and first version of README
</commit_message>
<xml_diff>
--- a/grading-rahm-homicide-rate/grading-rahm-homicide-rate.xlsx
+++ b/grading-rahm-homicide-rate/grading-rahm-homicide-rate.xlsx
@@ -17,13 +17,28 @@
     <t>key</t>
   </si>
   <si>
+    <t>state</t>
+  </si>
+  <si>
     <t>value</t>
+  </si>
+  <si>
+    <t>something</t>
   </si>
   <si>
     <t>headline</t>
   </si>
   <si>
+    <t>another_thing</t>
+  </si>
+  <si>
+    <t>Alabama</t>
+  </si>
+  <si>
     <t>The Headline For This Graphic</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
   <si>
     <t>subhed</t>
@@ -33,48 +48,6 @@
   </si>
   <si>
     <t>footnote</t>
-  </si>
-  <si>
-    <t>source</t>
-  </si>
-  <si>
-    <t>credit</t>
-  </si>
-  <si>
-    <t>NPR</t>
-  </si>
-  <si>
-    <t>hdr_state</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>hdr_something</t>
-  </si>
-  <si>
-    <t>Something</t>
-  </si>
-  <si>
-    <t>hdr_another_thing</t>
-  </si>
-  <si>
-    <t>Another Thing</t>
-  </si>
-  <si>
-    <t>state</t>
-  </si>
-  <si>
-    <t>something</t>
-  </si>
-  <si>
-    <t>another_thing</t>
-  </si>
-  <si>
-    <t>Alabama</t>
-  </si>
-  <si>
-    <t>2</t>
   </si>
   <si>
     <t>1819</t>
@@ -87,6 +60,9 @@
   </si>
   <si>
     <t>1958</t>
+  </si>
+  <si>
+    <t>source</t>
   </si>
   <si>
     <t>Arizona</t>
@@ -104,7 +80,13 @@
     <t>8</t>
   </si>
   <si>
+    <t>credit</t>
+  </si>
+  <si>
     <t>1836</t>
+  </si>
+  <si>
+    <t>NPR</t>
   </si>
   <si>
     <t>California</t>
@@ -133,6 +115,24 @@
   <si>
     <t>1788</t>
   </si>
+  <si>
+    <t>hdr_state</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>hdr_something</t>
+  </si>
+  <si>
+    <t>Something</t>
+  </si>
+  <si>
+    <t>hdr_another_thing</t>
+  </si>
+  <si>
+    <t>Another Thing</t>
+  </si>
 </sst>
 </file>
 
@@ -148,10 +148,10 @@
       <sz val="14.0"/>
     </font>
     <font>
-      <sz val="14.0"/>
+      <b/>
     </font>
     <font>
-      <b/>
+      <sz val="14.0"/>
     </font>
     <font/>
   </fonts>
@@ -186,24 +186,24 @@
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="2">
+      <alignment/>
+    </xf>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="2">
+      <alignment/>
+    </xf>
+    <xf fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="2"/>
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="3">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="2">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="3">
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="4">
       <alignment/>
     </xf>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="3">
-      <alignment/>
-    </xf>
-    <xf fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="3"/>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="4">
-      <alignment/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="4">
       <alignment/>
@@ -242,592 +242,592 @@
         <v>0</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>1</v>
-      </c>
-      <c s="2" r="C1"/>
-      <c s="2" r="D1"/>
-      <c s="2" r="E1"/>
-      <c s="2" r="F1"/>
-      <c s="2" r="G1"/>
-      <c s="2" r="H1"/>
-      <c s="2" r="I1"/>
-      <c s="2" r="J1"/>
-      <c s="2" r="K1"/>
-      <c s="2" r="L1"/>
-      <c s="2" r="M1"/>
-      <c s="2" r="N1"/>
-      <c s="2" r="O1"/>
-      <c s="2" r="P1"/>
-      <c s="2" r="Q1"/>
-      <c s="2" r="R1"/>
-      <c s="2" r="S1"/>
-      <c s="2" r="T1"/>
-      <c s="2" r="U1"/>
-      <c s="2" r="V1"/>
-      <c s="2" r="W1"/>
-      <c s="2" r="X1"/>
-      <c s="2" r="Y1"/>
-      <c s="2" r="Z1"/>
-    </row>
-    <row customHeight="1" r="2" ht="33.0">
-      <c t="s" s="3" r="A2">
         <v>2</v>
       </c>
-      <c t="s" s="3" r="B2">
-        <v>3</v>
-      </c>
-      <c s="4" r="C2"/>
-      <c s="4" r="D2"/>
-      <c s="4" r="E2"/>
-      <c s="4" r="F2"/>
-      <c s="4" r="G2"/>
-      <c s="4" r="H2"/>
-      <c s="4" r="I2"/>
-      <c s="4" r="J2"/>
-      <c s="4" r="K2"/>
-      <c s="4" r="L2"/>
-      <c s="4" r="M2"/>
-      <c s="4" r="N2"/>
-      <c s="4" r="O2"/>
-      <c s="4" r="P2"/>
-      <c s="4" r="Q2"/>
-      <c s="4" r="R2"/>
-      <c s="4" r="S2"/>
-      <c s="4" r="T2"/>
-      <c s="4" r="U2"/>
-      <c s="4" r="V2"/>
-      <c s="4" r="W2"/>
-      <c s="4" r="X2"/>
-      <c s="4" r="Y2"/>
-      <c s="4" r="Z2"/>
-    </row>
-    <row customHeight="1" r="3" ht="33.0">
-      <c t="s" s="3" r="A3">
+      <c s="3" r="C1"/>
+      <c s="3" r="D1"/>
+      <c s="3" r="E1"/>
+      <c s="3" r="F1"/>
+      <c s="3" r="G1"/>
+      <c s="3" r="H1"/>
+      <c s="3" r="I1"/>
+      <c s="3" r="J1"/>
+      <c s="3" r="K1"/>
+      <c s="3" r="L1"/>
+      <c s="3" r="M1"/>
+      <c s="3" r="N1"/>
+      <c s="3" r="O1"/>
+      <c s="3" r="P1"/>
+      <c s="3" r="Q1"/>
+      <c s="3" r="R1"/>
+      <c s="3" r="S1"/>
+      <c s="3" r="T1"/>
+      <c s="3" r="U1"/>
+      <c s="3" r="V1"/>
+      <c s="3" r="W1"/>
+      <c s="3" r="X1"/>
+      <c s="3" r="Y1"/>
+      <c s="3" r="Z1"/>
+    </row>
+    <row customHeight="1" r="2" ht="33.0">
+      <c t="s" s="6" r="A2">
         <v>4</v>
       </c>
-      <c t="s" s="3" r="B3">
-        <v>5</v>
-      </c>
-      <c s="4" r="C3"/>
-      <c s="4" r="D3"/>
-      <c s="4" r="E3"/>
-      <c s="4" r="F3"/>
-      <c s="4" r="G3"/>
-      <c s="4" r="H3"/>
-      <c s="4" r="I3"/>
-      <c s="4" r="J3"/>
-      <c s="4" r="K3"/>
-      <c s="4" r="L3"/>
-      <c s="4" r="M3"/>
-      <c s="4" r="N3"/>
-      <c s="4" r="O3"/>
-      <c s="4" r="P3"/>
-      <c s="4" r="Q3"/>
-      <c s="4" r="R3"/>
-      <c s="4" r="S3"/>
-      <c s="4" r="T3"/>
-      <c s="4" r="U3"/>
-      <c s="4" r="V3"/>
-      <c s="4" r="W3"/>
-      <c s="4" r="X3"/>
-      <c s="4" r="Y3"/>
-      <c s="4" r="Z3"/>
-    </row>
-    <row customHeight="1" r="4" ht="33.0">
-      <c t="s" s="3" r="A4">
-        <v>6</v>
-      </c>
-      <c s="3" r="B4"/>
-      <c s="4" r="C4"/>
-      <c s="4" r="D4"/>
-      <c s="4" r="E4"/>
-      <c s="4" r="F4"/>
-      <c s="4" r="G4"/>
-      <c s="4" r="H4"/>
-      <c s="4" r="I4"/>
-      <c s="4" r="J4"/>
-      <c s="4" r="K4"/>
-      <c s="4" r="L4"/>
-      <c s="4" r="M4"/>
-      <c s="4" r="N4"/>
-      <c s="4" r="O4"/>
-      <c s="4" r="P4"/>
-      <c s="4" r="Q4"/>
-      <c s="4" r="R4"/>
-      <c s="4" r="S4"/>
-      <c s="4" r="T4"/>
-      <c s="4" r="U4"/>
-      <c s="4" r="V4"/>
-      <c s="4" r="W4"/>
-      <c s="4" r="X4"/>
-      <c s="4" r="Y4"/>
-      <c s="4" r="Z4"/>
-    </row>
-    <row customHeight="1" r="5" ht="33.0">
-      <c t="s" s="3" r="A5">
+      <c t="s" s="6" r="B2">
         <v>7</v>
       </c>
-      <c s="3" r="B5"/>
-      <c s="4" r="C5"/>
-      <c s="4" r="D5"/>
-      <c s="4" r="E5"/>
-      <c s="4" r="F5"/>
-      <c s="4" r="G5"/>
-      <c s="4" r="H5"/>
-      <c s="4" r="I5"/>
-      <c s="4" r="J5"/>
-      <c s="4" r="K5"/>
-      <c s="4" r="L5"/>
-      <c s="4" r="M5"/>
-      <c s="4" r="N5"/>
-      <c s="4" r="O5"/>
-      <c s="4" r="P5"/>
-      <c s="4" r="Q5"/>
-      <c s="4" r="R5"/>
-      <c s="4" r="S5"/>
-      <c s="4" r="T5"/>
-      <c s="4" r="U5"/>
-      <c s="4" r="V5"/>
-      <c s="4" r="W5"/>
-      <c s="4" r="X5"/>
-      <c s="4" r="Y5"/>
-      <c s="4" r="Z5"/>
-    </row>
-    <row customHeight="1" r="6" ht="33.0">
-      <c t="s" s="3" r="A6">
-        <v>8</v>
-      </c>
-      <c t="s" s="3" r="B6">
+      <c s="8" r="C2"/>
+      <c s="8" r="D2"/>
+      <c s="8" r="E2"/>
+      <c s="8" r="F2"/>
+      <c s="8" r="G2"/>
+      <c s="8" r="H2"/>
+      <c s="8" r="I2"/>
+      <c s="8" r="J2"/>
+      <c s="8" r="K2"/>
+      <c s="8" r="L2"/>
+      <c s="8" r="M2"/>
+      <c s="8" r="N2"/>
+      <c s="8" r="O2"/>
+      <c s="8" r="P2"/>
+      <c s="8" r="Q2"/>
+      <c s="8" r="R2"/>
+      <c s="8" r="S2"/>
+      <c s="8" r="T2"/>
+      <c s="8" r="U2"/>
+      <c s="8" r="V2"/>
+      <c s="8" r="W2"/>
+      <c s="8" r="X2"/>
+      <c s="8" r="Y2"/>
+      <c s="8" r="Z2"/>
+    </row>
+    <row customHeight="1" r="3" ht="33.0">
+      <c t="s" s="6" r="A3">
         <v>9</v>
       </c>
-      <c s="4" r="C6"/>
-      <c s="4" r="D6"/>
-      <c s="4" r="E6"/>
-      <c s="4" r="F6"/>
-      <c s="4" r="G6"/>
-      <c s="4" r="H6"/>
-      <c s="4" r="I6"/>
-      <c s="4" r="J6"/>
-      <c s="4" r="K6"/>
-      <c s="4" r="L6"/>
-      <c s="4" r="M6"/>
-      <c s="4" r="N6"/>
-      <c s="4" r="O6"/>
-      <c s="4" r="P6"/>
-      <c s="4" r="Q6"/>
-      <c s="4" r="R6"/>
-      <c s="4" r="S6"/>
-      <c s="4" r="T6"/>
-      <c s="4" r="U6"/>
-      <c s="4" r="V6"/>
-      <c s="4" r="W6"/>
-      <c s="4" r="X6"/>
-      <c s="4" r="Y6"/>
-      <c s="4" r="Z6"/>
-    </row>
-    <row customHeight="1" r="7" ht="33.0">
-      <c s="4" r="A7"/>
-      <c s="4" r="B7"/>
-      <c s="4" r="C7"/>
-      <c s="4" r="D7"/>
-      <c s="4" r="E7"/>
-      <c s="4" r="F7"/>
-      <c s="4" r="G7"/>
-      <c s="4" r="H7"/>
-      <c s="4" r="I7"/>
-      <c s="4" r="J7"/>
-      <c s="4" r="K7"/>
-      <c s="4" r="L7"/>
-      <c s="4" r="M7"/>
-      <c s="4" r="N7"/>
-      <c s="4" r="O7"/>
-      <c s="4" r="P7"/>
-      <c s="4" r="Q7"/>
-      <c s="4" r="R7"/>
-      <c s="4" r="S7"/>
-      <c s="4" r="T7"/>
-      <c s="4" r="U7"/>
-      <c s="4" r="V7"/>
-      <c s="4" r="W7"/>
-      <c s="4" r="X7"/>
-      <c s="4" r="Y7"/>
-      <c s="4" r="Z7"/>
-    </row>
-    <row customHeight="1" r="8" ht="33.0">
-      <c t="s" s="3" r="A8">
+      <c t="s" s="6" r="B3">
         <v>10</v>
       </c>
-      <c t="s" s="3" r="B8">
+      <c s="8" r="C3"/>
+      <c s="8" r="D3"/>
+      <c s="8" r="E3"/>
+      <c s="8" r="F3"/>
+      <c s="8" r="G3"/>
+      <c s="8" r="H3"/>
+      <c s="8" r="I3"/>
+      <c s="8" r="J3"/>
+      <c s="8" r="K3"/>
+      <c s="8" r="L3"/>
+      <c s="8" r="M3"/>
+      <c s="8" r="N3"/>
+      <c s="8" r="O3"/>
+      <c s="8" r="P3"/>
+      <c s="8" r="Q3"/>
+      <c s="8" r="R3"/>
+      <c s="8" r="S3"/>
+      <c s="8" r="T3"/>
+      <c s="8" r="U3"/>
+      <c s="8" r="V3"/>
+      <c s="8" r="W3"/>
+      <c s="8" r="X3"/>
+      <c s="8" r="Y3"/>
+      <c s="8" r="Z3"/>
+    </row>
+    <row customHeight="1" r="4" ht="33.0">
+      <c t="s" s="6" r="A4">
         <v>11</v>
       </c>
-      <c s="4" r="C8"/>
-      <c s="4" r="D8"/>
-      <c s="4" r="E8"/>
-      <c s="4" r="F8"/>
-      <c s="4" r="G8"/>
-      <c s="4" r="H8"/>
-      <c s="4" r="I8"/>
-      <c s="4" r="J8"/>
-      <c s="4" r="K8"/>
-      <c s="4" r="L8"/>
-      <c s="4" r="M8"/>
-      <c s="4" r="N8"/>
-      <c s="4" r="O8"/>
-      <c s="4" r="P8"/>
-      <c s="4" r="Q8"/>
-      <c s="4" r="R8"/>
-      <c s="4" r="S8"/>
-      <c s="4" r="T8"/>
-      <c s="4" r="U8"/>
-      <c s="4" r="V8"/>
-      <c s="4" r="W8"/>
-      <c s="4" r="X8"/>
-      <c s="4" r="Y8"/>
-      <c s="4" r="Z8"/>
+      <c s="6" r="B4"/>
+      <c s="8" r="C4"/>
+      <c s="8" r="D4"/>
+      <c s="8" r="E4"/>
+      <c s="8" r="F4"/>
+      <c s="8" r="G4"/>
+      <c s="8" r="H4"/>
+      <c s="8" r="I4"/>
+      <c s="8" r="J4"/>
+      <c s="8" r="K4"/>
+      <c s="8" r="L4"/>
+      <c s="8" r="M4"/>
+      <c s="8" r="N4"/>
+      <c s="8" r="O4"/>
+      <c s="8" r="P4"/>
+      <c s="8" r="Q4"/>
+      <c s="8" r="R4"/>
+      <c s="8" r="S4"/>
+      <c s="8" r="T4"/>
+      <c s="8" r="U4"/>
+      <c s="8" r="V4"/>
+      <c s="8" r="W4"/>
+      <c s="8" r="X4"/>
+      <c s="8" r="Y4"/>
+      <c s="8" r="Z4"/>
+    </row>
+    <row customHeight="1" r="5" ht="33.0">
+      <c t="s" s="6" r="A5">
+        <v>16</v>
+      </c>
+      <c s="6" r="B5"/>
+      <c s="8" r="C5"/>
+      <c s="8" r="D5"/>
+      <c s="8" r="E5"/>
+      <c s="8" r="F5"/>
+      <c s="8" r="G5"/>
+      <c s="8" r="H5"/>
+      <c s="8" r="I5"/>
+      <c s="8" r="J5"/>
+      <c s="8" r="K5"/>
+      <c s="8" r="L5"/>
+      <c s="8" r="M5"/>
+      <c s="8" r="N5"/>
+      <c s="8" r="O5"/>
+      <c s="8" r="P5"/>
+      <c s="8" r="Q5"/>
+      <c s="8" r="R5"/>
+      <c s="8" r="S5"/>
+      <c s="8" r="T5"/>
+      <c s="8" r="U5"/>
+      <c s="8" r="V5"/>
+      <c s="8" r="W5"/>
+      <c s="8" r="X5"/>
+      <c s="8" r="Y5"/>
+      <c s="8" r="Z5"/>
+    </row>
+    <row customHeight="1" r="6" ht="33.0">
+      <c t="s" s="6" r="A6">
+        <v>22</v>
+      </c>
+      <c t="s" s="6" r="B6">
+        <v>24</v>
+      </c>
+      <c s="8" r="C6"/>
+      <c s="8" r="D6"/>
+      <c s="8" r="E6"/>
+      <c s="8" r="F6"/>
+      <c s="8" r="G6"/>
+      <c s="8" r="H6"/>
+      <c s="8" r="I6"/>
+      <c s="8" r="J6"/>
+      <c s="8" r="K6"/>
+      <c s="8" r="L6"/>
+      <c s="8" r="M6"/>
+      <c s="8" r="N6"/>
+      <c s="8" r="O6"/>
+      <c s="8" r="P6"/>
+      <c s="8" r="Q6"/>
+      <c s="8" r="R6"/>
+      <c s="8" r="S6"/>
+      <c s="8" r="T6"/>
+      <c s="8" r="U6"/>
+      <c s="8" r="V6"/>
+      <c s="8" r="W6"/>
+      <c s="8" r="X6"/>
+      <c s="8" r="Y6"/>
+      <c s="8" r="Z6"/>
+    </row>
+    <row customHeight="1" r="7" ht="33.0">
+      <c s="8" r="A7"/>
+      <c s="8" r="B7"/>
+      <c s="8" r="C7"/>
+      <c s="8" r="D7"/>
+      <c s="8" r="E7"/>
+      <c s="8" r="F7"/>
+      <c s="8" r="G7"/>
+      <c s="8" r="H7"/>
+      <c s="8" r="I7"/>
+      <c s="8" r="J7"/>
+      <c s="8" r="K7"/>
+      <c s="8" r="L7"/>
+      <c s="8" r="M7"/>
+      <c s="8" r="N7"/>
+      <c s="8" r="O7"/>
+      <c s="8" r="P7"/>
+      <c s="8" r="Q7"/>
+      <c s="8" r="R7"/>
+      <c s="8" r="S7"/>
+      <c s="8" r="T7"/>
+      <c s="8" r="U7"/>
+      <c s="8" r="V7"/>
+      <c s="8" r="W7"/>
+      <c s="8" r="X7"/>
+      <c s="8" r="Y7"/>
+      <c s="8" r="Z7"/>
+    </row>
+    <row customHeight="1" r="8" ht="33.0">
+      <c t="s" s="6" r="A8">
+        <v>34</v>
+      </c>
+      <c t="s" s="6" r="B8">
+        <v>35</v>
+      </c>
+      <c s="8" r="C8"/>
+      <c s="8" r="D8"/>
+      <c s="8" r="E8"/>
+      <c s="8" r="F8"/>
+      <c s="8" r="G8"/>
+      <c s="8" r="H8"/>
+      <c s="8" r="I8"/>
+      <c s="8" r="J8"/>
+      <c s="8" r="K8"/>
+      <c s="8" r="L8"/>
+      <c s="8" r="M8"/>
+      <c s="8" r="N8"/>
+      <c s="8" r="O8"/>
+      <c s="8" r="P8"/>
+      <c s="8" r="Q8"/>
+      <c s="8" r="R8"/>
+      <c s="8" r="S8"/>
+      <c s="8" r="T8"/>
+      <c s="8" r="U8"/>
+      <c s="8" r="V8"/>
+      <c s="8" r="W8"/>
+      <c s="8" r="X8"/>
+      <c s="8" r="Y8"/>
+      <c s="8" r="Z8"/>
     </row>
     <row customHeight="1" r="9" ht="33.0">
-      <c t="s" s="3" r="A9">
-        <v>12</v>
+      <c t="s" s="6" r="A9">
+        <v>36</v>
       </c>
-      <c t="s" s="3" r="B9">
-        <v>13</v>
+      <c t="s" s="6" r="B9">
+        <v>37</v>
       </c>
-      <c s="4" r="C9"/>
-      <c s="4" r="D9"/>
-      <c s="4" r="E9"/>
-      <c s="4" r="F9"/>
-      <c s="4" r="G9"/>
-      <c s="4" r="H9"/>
-      <c s="4" r="I9"/>
-      <c s="4" r="J9"/>
-      <c s="4" r="K9"/>
-      <c s="4" r="L9"/>
-      <c s="4" r="M9"/>
-      <c s="4" r="N9"/>
-      <c s="4" r="O9"/>
-      <c s="4" r="P9"/>
-      <c s="4" r="Q9"/>
-      <c s="4" r="R9"/>
-      <c s="4" r="S9"/>
-      <c s="4" r="T9"/>
-      <c s="4" r="U9"/>
-      <c s="4" r="V9"/>
-      <c s="4" r="W9"/>
-      <c s="4" r="X9"/>
-      <c s="4" r="Y9"/>
-      <c s="4" r="Z9"/>
+      <c s="8" r="C9"/>
+      <c s="8" r="D9"/>
+      <c s="8" r="E9"/>
+      <c s="8" r="F9"/>
+      <c s="8" r="G9"/>
+      <c s="8" r="H9"/>
+      <c s="8" r="I9"/>
+      <c s="8" r="J9"/>
+      <c s="8" r="K9"/>
+      <c s="8" r="L9"/>
+      <c s="8" r="M9"/>
+      <c s="8" r="N9"/>
+      <c s="8" r="O9"/>
+      <c s="8" r="P9"/>
+      <c s="8" r="Q9"/>
+      <c s="8" r="R9"/>
+      <c s="8" r="S9"/>
+      <c s="8" r="T9"/>
+      <c s="8" r="U9"/>
+      <c s="8" r="V9"/>
+      <c s="8" r="W9"/>
+      <c s="8" r="X9"/>
+      <c s="8" r="Y9"/>
+      <c s="8" r="Z9"/>
     </row>
     <row customHeight="1" r="10" ht="33.0">
-      <c t="s" s="3" r="A10">
-        <v>14</v>
+      <c t="s" s="6" r="A10">
+        <v>38</v>
       </c>
-      <c t="s" s="3" r="B10">
-        <v>15</v>
+      <c t="s" s="6" r="B10">
+        <v>39</v>
       </c>
-      <c s="4" r="C10"/>
-      <c s="4" r="D10"/>
-      <c s="4" r="E10"/>
-      <c s="4" r="F10"/>
-      <c s="4" r="G10"/>
-      <c s="4" r="H10"/>
-      <c s="4" r="I10"/>
-      <c s="4" r="J10"/>
-      <c s="4" r="K10"/>
-      <c s="4" r="L10"/>
-      <c s="4" r="M10"/>
-      <c s="4" r="N10"/>
-      <c s="4" r="O10"/>
-      <c s="4" r="P10"/>
-      <c s="4" r="Q10"/>
-      <c s="4" r="R10"/>
-      <c s="4" r="S10"/>
-      <c s="4" r="T10"/>
-      <c s="4" r="U10"/>
-      <c s="4" r="V10"/>
-      <c s="4" r="W10"/>
-      <c s="4" r="X10"/>
-      <c s="4" r="Y10"/>
-      <c s="4" r="Z10"/>
+      <c s="8" r="C10"/>
+      <c s="8" r="D10"/>
+      <c s="8" r="E10"/>
+      <c s="8" r="F10"/>
+      <c s="8" r="G10"/>
+      <c s="8" r="H10"/>
+      <c s="8" r="I10"/>
+      <c s="8" r="J10"/>
+      <c s="8" r="K10"/>
+      <c s="8" r="L10"/>
+      <c s="8" r="M10"/>
+      <c s="8" r="N10"/>
+      <c s="8" r="O10"/>
+      <c s="8" r="P10"/>
+      <c s="8" r="Q10"/>
+      <c s="8" r="R10"/>
+      <c s="8" r="S10"/>
+      <c s="8" r="T10"/>
+      <c s="8" r="U10"/>
+      <c s="8" r="V10"/>
+      <c s="8" r="W10"/>
+      <c s="8" r="X10"/>
+      <c s="8" r="Y10"/>
+      <c s="8" r="Z10"/>
     </row>
     <row customHeight="1" r="11" ht="33.0">
-      <c s="4" r="A11"/>
-      <c s="4" r="B11"/>
-      <c s="4" r="C11"/>
-      <c s="4" r="D11"/>
-      <c s="4" r="E11"/>
-      <c s="4" r="F11"/>
-      <c s="4" r="G11"/>
-      <c s="4" r="H11"/>
-      <c s="4" r="I11"/>
-      <c s="4" r="J11"/>
-      <c s="4" r="K11"/>
-      <c s="4" r="L11"/>
-      <c s="4" r="M11"/>
-      <c s="4" r="N11"/>
-      <c s="4" r="O11"/>
-      <c s="4" r="P11"/>
-      <c s="4" r="Q11"/>
-      <c s="4" r="R11"/>
-      <c s="4" r="S11"/>
-      <c s="4" r="T11"/>
-      <c s="4" r="U11"/>
-      <c s="4" r="V11"/>
-      <c s="4" r="W11"/>
-      <c s="4" r="X11"/>
-      <c s="4" r="Y11"/>
-      <c s="4" r="Z11"/>
+      <c s="8" r="A11"/>
+      <c s="8" r="B11"/>
+      <c s="8" r="C11"/>
+      <c s="8" r="D11"/>
+      <c s="8" r="E11"/>
+      <c s="8" r="F11"/>
+      <c s="8" r="G11"/>
+      <c s="8" r="H11"/>
+      <c s="8" r="I11"/>
+      <c s="8" r="J11"/>
+      <c s="8" r="K11"/>
+      <c s="8" r="L11"/>
+      <c s="8" r="M11"/>
+      <c s="8" r="N11"/>
+      <c s="8" r="O11"/>
+      <c s="8" r="P11"/>
+      <c s="8" r="Q11"/>
+      <c s="8" r="R11"/>
+      <c s="8" r="S11"/>
+      <c s="8" r="T11"/>
+      <c s="8" r="U11"/>
+      <c s="8" r="V11"/>
+      <c s="8" r="W11"/>
+      <c s="8" r="X11"/>
+      <c s="8" r="Y11"/>
+      <c s="8" r="Z11"/>
     </row>
     <row customHeight="1" r="12" ht="33.0">
-      <c s="4" r="A12"/>
-      <c s="4" r="B12"/>
-      <c s="4" r="C12"/>
-      <c s="4" r="D12"/>
-      <c s="4" r="E12"/>
-      <c s="4" r="F12"/>
-      <c s="4" r="G12"/>
-      <c s="4" r="H12"/>
-      <c s="4" r="I12"/>
-      <c s="4" r="J12"/>
-      <c s="4" r="K12"/>
-      <c s="4" r="L12"/>
-      <c s="4" r="M12"/>
-      <c s="4" r="N12"/>
-      <c s="4" r="O12"/>
-      <c s="4" r="P12"/>
-      <c s="4" r="Q12"/>
-      <c s="4" r="R12"/>
-      <c s="4" r="S12"/>
-      <c s="4" r="T12"/>
-      <c s="4" r="U12"/>
-      <c s="4" r="V12"/>
-      <c s="4" r="W12"/>
-      <c s="4" r="X12"/>
-      <c s="4" r="Y12"/>
-      <c s="4" r="Z12"/>
+      <c s="8" r="A12"/>
+      <c s="8" r="B12"/>
+      <c s="8" r="C12"/>
+      <c s="8" r="D12"/>
+      <c s="8" r="E12"/>
+      <c s="8" r="F12"/>
+      <c s="8" r="G12"/>
+      <c s="8" r="H12"/>
+      <c s="8" r="I12"/>
+      <c s="8" r="J12"/>
+      <c s="8" r="K12"/>
+      <c s="8" r="L12"/>
+      <c s="8" r="M12"/>
+      <c s="8" r="N12"/>
+      <c s="8" r="O12"/>
+      <c s="8" r="P12"/>
+      <c s="8" r="Q12"/>
+      <c s="8" r="R12"/>
+      <c s="8" r="S12"/>
+      <c s="8" r="T12"/>
+      <c s="8" r="U12"/>
+      <c s="8" r="V12"/>
+      <c s="8" r="W12"/>
+      <c s="8" r="X12"/>
+      <c s="8" r="Y12"/>
+      <c s="8" r="Z12"/>
     </row>
     <row customHeight="1" r="13" ht="33.0">
-      <c s="4" r="A13"/>
-      <c s="4" r="B13"/>
-      <c s="4" r="C13"/>
-      <c s="4" r="D13"/>
-      <c s="4" r="E13"/>
-      <c s="4" r="F13"/>
-      <c s="4" r="G13"/>
-      <c s="4" r="H13"/>
-      <c s="4" r="I13"/>
-      <c s="4" r="J13"/>
-      <c s="4" r="K13"/>
-      <c s="4" r="L13"/>
-      <c s="4" r="M13"/>
-      <c s="4" r="N13"/>
-      <c s="4" r="O13"/>
-      <c s="4" r="P13"/>
-      <c s="4" r="Q13"/>
-      <c s="4" r="R13"/>
-      <c s="4" r="S13"/>
-      <c s="4" r="T13"/>
-      <c s="4" r="U13"/>
-      <c s="4" r="V13"/>
-      <c s="4" r="W13"/>
-      <c s="4" r="X13"/>
-      <c s="4" r="Y13"/>
-      <c s="4" r="Z13"/>
+      <c s="8" r="A13"/>
+      <c s="8" r="B13"/>
+      <c s="8" r="C13"/>
+      <c s="8" r="D13"/>
+      <c s="8" r="E13"/>
+      <c s="8" r="F13"/>
+      <c s="8" r="G13"/>
+      <c s="8" r="H13"/>
+      <c s="8" r="I13"/>
+      <c s="8" r="J13"/>
+      <c s="8" r="K13"/>
+      <c s="8" r="L13"/>
+      <c s="8" r="M13"/>
+      <c s="8" r="N13"/>
+      <c s="8" r="O13"/>
+      <c s="8" r="P13"/>
+      <c s="8" r="Q13"/>
+      <c s="8" r="R13"/>
+      <c s="8" r="S13"/>
+      <c s="8" r="T13"/>
+      <c s="8" r="U13"/>
+      <c s="8" r="V13"/>
+      <c s="8" r="W13"/>
+      <c s="8" r="X13"/>
+      <c s="8" r="Y13"/>
+      <c s="8" r="Z13"/>
     </row>
     <row customHeight="1" r="14" ht="33.0">
-      <c s="4" r="A14"/>
-      <c s="4" r="B14"/>
-      <c s="4" r="C14"/>
-      <c s="4" r="D14"/>
-      <c s="4" r="E14"/>
-      <c s="4" r="F14"/>
-      <c s="4" r="G14"/>
-      <c s="4" r="H14"/>
-      <c s="4" r="I14"/>
-      <c s="4" r="J14"/>
-      <c s="4" r="K14"/>
-      <c s="4" r="L14"/>
-      <c s="4" r="M14"/>
-      <c s="4" r="N14"/>
-      <c s="4" r="O14"/>
-      <c s="4" r="P14"/>
-      <c s="4" r="Q14"/>
-      <c s="4" r="R14"/>
-      <c s="4" r="S14"/>
-      <c s="4" r="T14"/>
-      <c s="4" r="U14"/>
-      <c s="4" r="V14"/>
-      <c s="4" r="W14"/>
-      <c s="4" r="X14"/>
-      <c s="4" r="Y14"/>
-      <c s="4" r="Z14"/>
+      <c s="8" r="A14"/>
+      <c s="8" r="B14"/>
+      <c s="8" r="C14"/>
+      <c s="8" r="D14"/>
+      <c s="8" r="E14"/>
+      <c s="8" r="F14"/>
+      <c s="8" r="G14"/>
+      <c s="8" r="H14"/>
+      <c s="8" r="I14"/>
+      <c s="8" r="J14"/>
+      <c s="8" r="K14"/>
+      <c s="8" r="L14"/>
+      <c s="8" r="M14"/>
+      <c s="8" r="N14"/>
+      <c s="8" r="O14"/>
+      <c s="8" r="P14"/>
+      <c s="8" r="Q14"/>
+      <c s="8" r="R14"/>
+      <c s="8" r="S14"/>
+      <c s="8" r="T14"/>
+      <c s="8" r="U14"/>
+      <c s="8" r="V14"/>
+      <c s="8" r="W14"/>
+      <c s="8" r="X14"/>
+      <c s="8" r="Y14"/>
+      <c s="8" r="Z14"/>
     </row>
     <row customHeight="1" r="15" ht="33.0">
-      <c s="4" r="A15"/>
-      <c s="4" r="B15"/>
-      <c s="4" r="C15"/>
-      <c s="4" r="D15"/>
-      <c s="4" r="E15"/>
-      <c s="4" r="F15"/>
-      <c s="4" r="G15"/>
-      <c s="4" r="H15"/>
-      <c s="4" r="I15"/>
-      <c s="4" r="J15"/>
-      <c s="4" r="K15"/>
-      <c s="4" r="L15"/>
-      <c s="4" r="M15"/>
-      <c s="4" r="N15"/>
-      <c s="4" r="O15"/>
-      <c s="4" r="P15"/>
-      <c s="4" r="Q15"/>
-      <c s="4" r="R15"/>
-      <c s="4" r="S15"/>
-      <c s="4" r="T15"/>
-      <c s="4" r="U15"/>
-      <c s="4" r="V15"/>
-      <c s="4" r="W15"/>
-      <c s="4" r="X15"/>
-      <c s="4" r="Y15"/>
-      <c s="4" r="Z15"/>
+      <c s="8" r="A15"/>
+      <c s="8" r="B15"/>
+      <c s="8" r="C15"/>
+      <c s="8" r="D15"/>
+      <c s="8" r="E15"/>
+      <c s="8" r="F15"/>
+      <c s="8" r="G15"/>
+      <c s="8" r="H15"/>
+      <c s="8" r="I15"/>
+      <c s="8" r="J15"/>
+      <c s="8" r="K15"/>
+      <c s="8" r="L15"/>
+      <c s="8" r="M15"/>
+      <c s="8" r="N15"/>
+      <c s="8" r="O15"/>
+      <c s="8" r="P15"/>
+      <c s="8" r="Q15"/>
+      <c s="8" r="R15"/>
+      <c s="8" r="S15"/>
+      <c s="8" r="T15"/>
+      <c s="8" r="U15"/>
+      <c s="8" r="V15"/>
+      <c s="8" r="W15"/>
+      <c s="8" r="X15"/>
+      <c s="8" r="Y15"/>
+      <c s="8" r="Z15"/>
     </row>
     <row customHeight="1" r="16" ht="33.0">
-      <c s="4" r="A16"/>
-      <c s="4" r="B16"/>
-      <c s="4" r="C16"/>
-      <c s="4" r="D16"/>
-      <c s="4" r="E16"/>
-      <c s="4" r="F16"/>
-      <c s="4" r="G16"/>
-      <c s="4" r="H16"/>
-      <c s="4" r="I16"/>
-      <c s="4" r="J16"/>
-      <c s="4" r="K16"/>
-      <c s="4" r="L16"/>
-      <c s="4" r="M16"/>
-      <c s="4" r="N16"/>
-      <c s="4" r="O16"/>
-      <c s="4" r="P16"/>
-      <c s="4" r="Q16"/>
-      <c s="4" r="R16"/>
-      <c s="4" r="S16"/>
-      <c s="4" r="T16"/>
-      <c s="4" r="U16"/>
-      <c s="4" r="V16"/>
-      <c s="4" r="W16"/>
-      <c s="4" r="X16"/>
-      <c s="4" r="Y16"/>
-      <c s="4" r="Z16"/>
+      <c s="8" r="A16"/>
+      <c s="8" r="B16"/>
+      <c s="8" r="C16"/>
+      <c s="8" r="D16"/>
+      <c s="8" r="E16"/>
+      <c s="8" r="F16"/>
+      <c s="8" r="G16"/>
+      <c s="8" r="H16"/>
+      <c s="8" r="I16"/>
+      <c s="8" r="J16"/>
+      <c s="8" r="K16"/>
+      <c s="8" r="L16"/>
+      <c s="8" r="M16"/>
+      <c s="8" r="N16"/>
+      <c s="8" r="O16"/>
+      <c s="8" r="P16"/>
+      <c s="8" r="Q16"/>
+      <c s="8" r="R16"/>
+      <c s="8" r="S16"/>
+      <c s="8" r="T16"/>
+      <c s="8" r="U16"/>
+      <c s="8" r="V16"/>
+      <c s="8" r="W16"/>
+      <c s="8" r="X16"/>
+      <c s="8" r="Y16"/>
+      <c s="8" r="Z16"/>
     </row>
     <row customHeight="1" r="17" ht="33.0">
-      <c s="4" r="A17"/>
-      <c s="4" r="B17"/>
-      <c s="4" r="C17"/>
-      <c s="4" r="D17"/>
-      <c s="4" r="E17"/>
-      <c s="4" r="F17"/>
-      <c s="4" r="G17"/>
-      <c s="4" r="H17"/>
-      <c s="4" r="I17"/>
-      <c s="4" r="J17"/>
-      <c s="4" r="K17"/>
-      <c s="4" r="L17"/>
-      <c s="4" r="M17"/>
-      <c s="4" r="N17"/>
-      <c s="4" r="O17"/>
-      <c s="4" r="P17"/>
-      <c s="4" r="Q17"/>
-      <c s="4" r="R17"/>
-      <c s="4" r="S17"/>
-      <c s="4" r="T17"/>
-      <c s="4" r="U17"/>
-      <c s="4" r="V17"/>
-      <c s="4" r="W17"/>
-      <c s="4" r="X17"/>
-      <c s="4" r="Y17"/>
-      <c s="4" r="Z17"/>
+      <c s="8" r="A17"/>
+      <c s="8" r="B17"/>
+      <c s="8" r="C17"/>
+      <c s="8" r="D17"/>
+      <c s="8" r="E17"/>
+      <c s="8" r="F17"/>
+      <c s="8" r="G17"/>
+      <c s="8" r="H17"/>
+      <c s="8" r="I17"/>
+      <c s="8" r="J17"/>
+      <c s="8" r="K17"/>
+      <c s="8" r="L17"/>
+      <c s="8" r="M17"/>
+      <c s="8" r="N17"/>
+      <c s="8" r="O17"/>
+      <c s="8" r="P17"/>
+      <c s="8" r="Q17"/>
+      <c s="8" r="R17"/>
+      <c s="8" r="S17"/>
+      <c s="8" r="T17"/>
+      <c s="8" r="U17"/>
+      <c s="8" r="V17"/>
+      <c s="8" r="W17"/>
+      <c s="8" r="X17"/>
+      <c s="8" r="Y17"/>
+      <c s="8" r="Z17"/>
     </row>
     <row customHeight="1" r="18" ht="33.0">
-      <c s="4" r="A18"/>
-      <c s="4" r="B18"/>
-      <c s="4" r="C18"/>
-      <c s="4" r="D18"/>
-      <c s="4" r="E18"/>
-      <c s="4" r="F18"/>
-      <c s="4" r="G18"/>
-      <c s="4" r="H18"/>
-      <c s="4" r="I18"/>
-      <c s="4" r="J18"/>
-      <c s="4" r="K18"/>
-      <c s="4" r="L18"/>
-      <c s="4" r="M18"/>
-      <c s="4" r="N18"/>
-      <c s="4" r="O18"/>
-      <c s="4" r="P18"/>
-      <c s="4" r="Q18"/>
-      <c s="4" r="R18"/>
-      <c s="4" r="S18"/>
-      <c s="4" r="T18"/>
-      <c s="4" r="U18"/>
-      <c s="4" r="V18"/>
-      <c s="4" r="W18"/>
-      <c s="4" r="X18"/>
-      <c s="4" r="Y18"/>
-      <c s="4" r="Z18"/>
+      <c s="8" r="A18"/>
+      <c s="8" r="B18"/>
+      <c s="8" r="C18"/>
+      <c s="8" r="D18"/>
+      <c s="8" r="E18"/>
+      <c s="8" r="F18"/>
+      <c s="8" r="G18"/>
+      <c s="8" r="H18"/>
+      <c s="8" r="I18"/>
+      <c s="8" r="J18"/>
+      <c s="8" r="K18"/>
+      <c s="8" r="L18"/>
+      <c s="8" r="M18"/>
+      <c s="8" r="N18"/>
+      <c s="8" r="O18"/>
+      <c s="8" r="P18"/>
+      <c s="8" r="Q18"/>
+      <c s="8" r="R18"/>
+      <c s="8" r="S18"/>
+      <c s="8" r="T18"/>
+      <c s="8" r="U18"/>
+      <c s="8" r="V18"/>
+      <c s="8" r="W18"/>
+      <c s="8" r="X18"/>
+      <c s="8" r="Y18"/>
+      <c s="8" r="Z18"/>
     </row>
     <row customHeight="1" r="19" ht="33.0">
-      <c s="4" r="A19"/>
-      <c s="4" r="B19"/>
-      <c s="4" r="C19"/>
-      <c s="4" r="D19"/>
-      <c s="4" r="E19"/>
-      <c s="4" r="F19"/>
-      <c s="4" r="G19"/>
-      <c s="4" r="H19"/>
-      <c s="4" r="I19"/>
-      <c s="4" r="J19"/>
-      <c s="4" r="K19"/>
-      <c s="4" r="L19"/>
-      <c s="4" r="M19"/>
-      <c s="4" r="N19"/>
-      <c s="4" r="O19"/>
-      <c s="4" r="P19"/>
-      <c s="4" r="Q19"/>
-      <c s="4" r="R19"/>
-      <c s="4" r="S19"/>
-      <c s="4" r="T19"/>
-      <c s="4" r="U19"/>
-      <c s="4" r="V19"/>
-      <c s="4" r="W19"/>
-      <c s="4" r="X19"/>
-      <c s="4" r="Y19"/>
-      <c s="4" r="Z19"/>
+      <c s="8" r="A19"/>
+      <c s="8" r="B19"/>
+      <c s="8" r="C19"/>
+      <c s="8" r="D19"/>
+      <c s="8" r="E19"/>
+      <c s="8" r="F19"/>
+      <c s="8" r="G19"/>
+      <c s="8" r="H19"/>
+      <c s="8" r="I19"/>
+      <c s="8" r="J19"/>
+      <c s="8" r="K19"/>
+      <c s="8" r="L19"/>
+      <c s="8" r="M19"/>
+      <c s="8" r="N19"/>
+      <c s="8" r="O19"/>
+      <c s="8" r="P19"/>
+      <c s="8" r="Q19"/>
+      <c s="8" r="R19"/>
+      <c s="8" r="S19"/>
+      <c s="8" r="T19"/>
+      <c s="8" r="U19"/>
+      <c s="8" r="V19"/>
+      <c s="8" r="W19"/>
+      <c s="8" r="X19"/>
+      <c s="8" r="Y19"/>
+      <c s="8" r="Z19"/>
     </row>
     <row customHeight="1" r="20" ht="33.0">
-      <c s="4" r="A20"/>
-      <c s="4" r="B20"/>
-      <c s="4" r="C20"/>
-      <c s="4" r="D20"/>
-      <c s="4" r="E20"/>
-      <c s="4" r="F20"/>
-      <c s="4" r="G20"/>
-      <c s="4" r="H20"/>
-      <c s="4" r="I20"/>
-      <c s="4" r="J20"/>
-      <c s="4" r="K20"/>
-      <c s="4" r="L20"/>
-      <c s="4" r="M20"/>
-      <c s="4" r="N20"/>
-      <c s="4" r="O20"/>
-      <c s="4" r="P20"/>
-      <c s="4" r="Q20"/>
-      <c s="4" r="R20"/>
-      <c s="4" r="S20"/>
-      <c s="4" r="T20"/>
-      <c s="4" r="U20"/>
-      <c s="4" r="V20"/>
-      <c s="4" r="W20"/>
-      <c s="4" r="X20"/>
-      <c s="4" r="Y20"/>
-      <c s="4" r="Z20"/>
+      <c s="8" r="A20"/>
+      <c s="8" r="B20"/>
+      <c s="8" r="C20"/>
+      <c s="8" r="D20"/>
+      <c s="8" r="E20"/>
+      <c s="8" r="F20"/>
+      <c s="8" r="G20"/>
+      <c s="8" r="H20"/>
+      <c s="8" r="I20"/>
+      <c s="8" r="J20"/>
+      <c s="8" r="K20"/>
+      <c s="8" r="L20"/>
+      <c s="8" r="M20"/>
+      <c s="8" r="N20"/>
+      <c s="8" r="O20"/>
+      <c s="8" r="P20"/>
+      <c s="8" r="Q20"/>
+      <c s="8" r="R20"/>
+      <c s="8" r="S20"/>
+      <c s="8" r="T20"/>
+      <c s="8" r="U20"/>
+      <c s="8" r="V20"/>
+      <c s="8" r="W20"/>
+      <c s="8" r="X20"/>
+      <c s="8" r="Y20"/>
+      <c s="8" r="Z20"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -842,114 +842,114 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c t="s" s="5" r="A1">
-        <v>16</v>
+      <c t="s" s="2" r="A1">
+        <v>1</v>
       </c>
-      <c t="s" s="6" r="B1">
+      <c t="s" s="4" r="B1">
+        <v>3</v>
+      </c>
+      <c t="s" s="4" r="C1">
+        <v>5</v>
+      </c>
+      <c s="5" r="D1"/>
+      <c s="5" r="E1"/>
+      <c s="5" r="F1"/>
+      <c s="5" r="G1"/>
+      <c s="5" r="H1"/>
+      <c s="5" r="I1"/>
+      <c s="5" r="J1"/>
+      <c s="5" r="K1"/>
+      <c s="5" r="L1"/>
+      <c s="5" r="M1"/>
+      <c s="5" r="N1"/>
+      <c s="5" r="O1"/>
+      <c s="5" r="P1"/>
+      <c s="5" r="Q1"/>
+      <c s="5" r="R1"/>
+      <c s="5" r="S1"/>
+      <c s="5" r="T1"/>
+      <c s="5" r="U1"/>
+      <c s="5" r="V1"/>
+      <c s="5" r="W1"/>
+      <c s="5" r="X1"/>
+      <c s="5" r="Y1"/>
+      <c s="5" r="Z1"/>
+    </row>
+    <row r="2">
+      <c t="s" s="7" r="A2">
+        <v>6</v>
+      </c>
+      <c t="s" s="9" r="B2">
+        <v>8</v>
+      </c>
+      <c t="s" s="9" r="C2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3">
+      <c t="s" s="7" r="A3">
+        <v>13</v>
+      </c>
+      <c t="s" s="9" r="B3">
+        <v>14</v>
+      </c>
+      <c t="s" s="9" r="C3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4">
+      <c t="s" s="7" r="A4">
         <v>17</v>
       </c>
-      <c t="s" s="6" r="C1">
+      <c t="s" s="9" r="B4">
         <v>18</v>
       </c>
-      <c s="7" r="D1"/>
-      <c s="7" r="E1"/>
-      <c s="7" r="F1"/>
-      <c s="7" r="G1"/>
-      <c s="7" r="H1"/>
-      <c s="7" r="I1"/>
-      <c s="7" r="J1"/>
-      <c s="7" r="K1"/>
-      <c s="7" r="L1"/>
-      <c s="7" r="M1"/>
-      <c s="7" r="N1"/>
-      <c s="7" r="O1"/>
-      <c s="7" r="P1"/>
-      <c s="7" r="Q1"/>
-      <c s="7" r="R1"/>
-      <c s="7" r="S1"/>
-      <c s="7" r="T1"/>
-      <c s="7" r="U1"/>
-      <c s="7" r="V1"/>
-      <c s="7" r="W1"/>
-      <c s="7" r="X1"/>
-      <c s="7" r="Y1"/>
-      <c s="7" r="Z1"/>
-    </row>
-    <row r="2">
-      <c t="s" s="8" r="A2">
+      <c t="s" s="9" r="C4">
         <v>19</v>
       </c>
-      <c t="s" s="9" r="B2">
+    </row>
+    <row r="5">
+      <c t="s" s="7" r="A5">
         <v>20</v>
       </c>
-      <c t="s" s="9" r="C2">
+      <c t="s" s="9" r="B5">
         <v>21</v>
       </c>
-    </row>
-    <row r="3">
-      <c t="s" s="8" r="A3">
-        <v>22</v>
-      </c>
-      <c t="s" s="9" r="B3">
+      <c t="s" s="9" r="C5">
         <v>23</v>
       </c>
-      <c t="s" s="9" r="C3">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4">
-      <c t="s" s="8" r="A4">
+    </row>
+    <row r="6">
+      <c t="s" s="7" r="A6">
         <v>25</v>
       </c>
-      <c t="s" s="9" r="B4">
+      <c t="s" s="9" r="B6">
         <v>26</v>
       </c>
-      <c t="s" s="9" r="C4">
+      <c t="s" s="9" r="C6">
         <v>27</v>
       </c>
     </row>
-    <row r="5">
-      <c t="s" s="8" r="A5">
+    <row r="7">
+      <c t="s" s="7" r="A7">
         <v>28</v>
       </c>
-      <c t="s" s="9" r="B5">
+      <c t="s" s="9" r="B7">
         <v>29</v>
       </c>
-      <c t="s" s="9" r="C5">
+      <c t="s" s="9" r="C7">
         <v>30</v>
       </c>
     </row>
-    <row r="6">
-      <c t="s" s="8" r="A6">
+    <row r="8">
+      <c t="s" s="7" r="A8">
         <v>31</v>
       </c>
-      <c t="s" s="9" r="B6">
+      <c t="s" s="9" r="B8">
         <v>32</v>
       </c>
-      <c t="s" s="9" r="C6">
+      <c t="s" s="9" r="C8">
         <v>33</v>
-      </c>
-    </row>
-    <row r="7">
-      <c t="s" s="8" r="A7">
-        <v>34</v>
-      </c>
-      <c t="s" s="9" r="B7">
-        <v>35</v>
-      </c>
-      <c t="s" s="9" r="C7">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8">
-      <c t="s" s="8" r="A8">
-        <v>37</v>
-      </c>
-      <c t="s" s="9" r="B8">
-        <v>38</v>
-      </c>
-      <c t="s" s="9" r="C8">
-        <v>39</v>
       </c>
     </row>
     <row r="9">

</xml_diff>